<commit_message>
Add multiple courses and labs at a time through importing
</commit_message>
<xml_diff>
--- a/src/assets/templates/course_template.xlsx
+++ b/src/assets/templates/course_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinhle/dev/typescript/lab-manamgement-web-v2/src/assets/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Downloads\Telegram Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6624C8-AF24-F540-A5F0-DE4974380796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F8E00-C1D7-4EC1-8A44-78008F533D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5863" yWindow="5040" windowWidth="26331" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>#</t>
   </si>
@@ -71,23 +71,290 @@
     <t>1</t>
   </si>
   <si>
-    <t>Big Data Analysis</t>
-  </si>
-  <si>
     <t>Theory</t>
   </si>
   <si>
     <t>Course ID</t>
   </si>
   <si>
-    <t>BDAN333977</t>
+    <t xml:space="preserve">Introduction to Information Technology </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>INPR130285E</t>
+  </si>
+  <si>
+    <t>Introduction to programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programming techniques </t>
+  </si>
+  <si>
+    <t>Discrete Mathematics and Graph Theory</t>
+  </si>
+  <si>
+    <t>DASA230179E</t>
+  </si>
+  <si>
+    <t>Data Structures and Algorithms</t>
+  </si>
+  <si>
+    <t>OOPR230279E</t>
+  </si>
+  <si>
+    <t>Object-Oriented Programming</t>
+  </si>
+  <si>
+    <t>WIPR230579E</t>
+  </si>
+  <si>
+    <t>Windows Programming</t>
+  </si>
+  <si>
+    <t>INSE330379E</t>
+  </si>
+  <si>
+    <t>Information Security</t>
+  </si>
+  <si>
+    <t>WEPR330479E</t>
+  </si>
+  <si>
+    <t>Web Programming</t>
+  </si>
+  <si>
+    <t>CAAL230180E</t>
+  </si>
+  <si>
+    <t>Computer Architecture and Assembly Languages</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>OPSY330280E</t>
+  </si>
+  <si>
+    <t>NEES330380E</t>
+  </si>
+  <si>
+    <t>DIGR230485E</t>
+  </si>
+  <si>
+    <t>PRTE230385E</t>
+  </si>
+  <si>
+    <t>INIT130185E</t>
+  </si>
+  <si>
+    <t>Networking  Essentials</t>
+  </si>
+  <si>
+    <t>DBSY230184E</t>
+  </si>
+  <si>
+    <t>Database Systems</t>
+  </si>
+  <si>
+    <t>DBMS330284E</t>
+  </si>
+  <si>
+    <t>Database Management Systems</t>
+  </si>
+  <si>
+    <t>CLCO432779E</t>
+  </si>
+  <si>
+    <t>Cloud computing</t>
+  </si>
+  <si>
+    <t>PROJ212779E</t>
+  </si>
+  <si>
+    <t>Project 1</t>
+  </si>
+  <si>
+    <t>PROJ212879E</t>
+  </si>
+  <si>
+    <t>Project 2</t>
+  </si>
+  <si>
+    <t>PROJ212979E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project 3 </t>
+  </si>
+  <si>
+    <t>IIOT431480E</t>
+  </si>
+  <si>
+    <t>Introduction to IoT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMHC333179E </t>
+  </si>
+  <si>
+    <t>Agile methods</t>
+  </si>
+  <si>
+    <t>GRPR423279E</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>SOEN330679E</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>OOSD330879E</t>
+  </si>
+  <si>
+    <t>Object-Oriented Software Design</t>
+  </si>
+  <si>
+    <t>MOPR331279E</t>
+  </si>
+  <si>
+    <t>Programming for Mobile Devices</t>
+  </si>
+  <si>
+    <t>SOTE431079E</t>
+  </si>
+  <si>
+    <t>Software Testing</t>
+  </si>
+  <si>
+    <t>MTSE431179E</t>
+  </si>
+  <si>
+    <t>Modern Technologies on Software Engineering</t>
+  </si>
+  <si>
+    <t>POSE431479E</t>
+  </si>
+  <si>
+    <t>Project on Software Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRPR401979E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capstone project </t>
+  </si>
+  <si>
+    <t>MOPL331379E</t>
+  </si>
+  <si>
+    <t>Advanced Programming Language</t>
+  </si>
+  <si>
+    <t>ESYS431080E</t>
+  </si>
+  <si>
+    <t>Embedded Systems</t>
+  </si>
+  <si>
+    <t>ITPM430884E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Technology Project Management </t>
+  </si>
+  <si>
+    <t>ECOM430984E</t>
+  </si>
+  <si>
+    <t>Electronic Commerce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WESE431479E </t>
+  </si>
+  <si>
+    <t>Web Security</t>
+  </si>
+  <si>
+    <t>SOPM431679E</t>
+  </si>
+  <si>
+    <t>Software project management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAP431779E </t>
+  </si>
+  <si>
+    <t>Web Services and Applications</t>
+  </si>
+  <si>
+    <t>ADMP431879E</t>
+  </si>
+  <si>
+    <t>Advanced Programming for Mobile Devices</t>
+  </si>
+  <si>
+    <t>NPRO430980E</t>
+  </si>
+  <si>
+    <t>Networks Programming</t>
+  </si>
+  <si>
+    <t>NMSY331180E</t>
+  </si>
+  <si>
+    <t>Network Monitoring Systems</t>
+  </si>
+  <si>
+    <t>WINE331480E</t>
+  </si>
+  <si>
+    <t>Wireless Networks</t>
+  </si>
+  <si>
+    <t>DAWH430784E</t>
+  </si>
+  <si>
+    <t>Data Warehouse</t>
+  </si>
+  <si>
+    <t>INRE431084E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Retrieval </t>
+  </si>
+  <si>
+    <t>ISAC431384E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information systems audit and control </t>
+  </si>
+  <si>
+    <t>SOIS431484E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special topics in IS </t>
+  </si>
+  <si>
+    <t>HCIN431979E</t>
+  </si>
+  <si>
+    <t>Human computer interaction</t>
+  </si>
+  <si>
+    <t>ESDN432079E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design of educational software </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,6 +398,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -195,19 +469,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,26 +823,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.35546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="53.35546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="5"/>
+    <col min="5" max="5" width="15.640625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -579,199 +856,916 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="3">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="3">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="3">
+        <v>3</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="3">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="3">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="3">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="3">
+        <v>3</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="3">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A58" s="2"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A60" s="2"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A62" s="2"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A63" s="2"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A65" s="2"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A66" s="2"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2 A1 D1:E1 C2 E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A2 A1 D1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>